<commit_message>
Dicionario de dados atualizado apos realizacao de mudancas no script 2 (fase2)
</commit_message>
<xml_diff>
--- a/DIcionario de Dados das Tabelas.xlsx
+++ b/DIcionario de Dados das Tabelas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vf_ga\OneDrive\Documentos\6Semestre\MegaDados\Projeto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vf_ga\OneDrive\Documentos\6Semestre\MegaDados\Porjeto1-GIT\MegadadosProjeto1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="91">
   <si>
     <t xml:space="preserve">Usuario </t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>nome da acao para entender qual foi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -408,9 +411,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,6 +418,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -700,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="M183" sqref="M183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,21 +723,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -874,21 +877,21 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="8"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -1099,21 +1102,21 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
@@ -1182,21 +1185,21 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
@@ -1290,21 +1293,21 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
@@ -1513,21 +1516,21 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
@@ -1627,21 +1630,21 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
@@ -1741,21 +1744,21 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="8"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="7"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
@@ -1908,21 +1911,21 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
-      <c r="M55" s="8"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
@@ -2040,6 +2043,11 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="183" spans="13:13" x14ac:dyDescent="0.35">
+      <c r="M183" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>